<commit_message>
fix typo + fix link to pin 6 no ejector for MUX
</commit_message>
<xml_diff>
--- a/sphinx/source/Ohmpi_V2_00/step_n_3/a/MUX_board_list_2_xx.xlsx
+++ b/sphinx/source/Ohmpi_V2_00/step_n_3/a/MUX_board_list_2_xx.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Component</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pin strip no ejector  6 pins</t>
+  </si>
+  <si>
+    <t>https://www.conrad.com/p/tru-components-1580990-pin-strip-no-ejector-contact-spacing-254-mm-total-number-of-pins-6-no-of-rows-2-1-pcs-1580990</t>
   </si>
   <si>
     <t xml:space="preserve">Dual screw terminal (5.08-mm pitch)</t>
@@ -330,15 +333,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <color indexed="63"/>
-      <sz val="10.000000"/>
-    </font>
-    <font>
       <name val="Calibri"/>
       <color theme="10"/>
       <sz val="11.000000"/>
       <u/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color indexed="63"/>
+      <sz val="10.000000"/>
     </font>
   </fonts>
   <fills count="33">
@@ -696,7 +699,7 @@
     <xf fontId="16" fillId="0" borderId="8" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1"/>
     <xf fontId="17" fillId="32" borderId="9" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -705,7 +708,8 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="30" applyFont="1"/>
+    <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="30" applyFont="1" applyAlignment="1">
@@ -714,7 +718,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="18" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Accent1" xfId="1" builtinId="30"/>
@@ -1387,15 +1391,15 @@
         <v>11</v>
       </c>
       <c r="F5" s="1">
-        <v>10120550</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>1580990</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6">
         <v>12</v>
@@ -1408,18 +1412,18 @@
         <v>7.7759999999999998</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>12</v>
@@ -1432,18 +1436,18 @@
         <v>2.46</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>16</v>
@@ -1456,18 +1460,18 @@
         <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="4">
+        <v>28</v>
+      </c>
+      <c r="F8" s="5">
         <v>732</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>256</v>
@@ -1480,18 +1484,18 @@
         <v>325.12</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>256</v>
@@ -1504,18 +1508,18 @@
         <v>120.57599999999999</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>256</v>
@@ -1528,18 +1532,18 @@
         <v>15.616</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B12">
         <v>4</v>
@@ -1551,19 +1555,19 @@
         <f t="shared" si="0"/>
         <v>23.559999999999999</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>42</v>
+      <c r="E12" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="F12" s="1">
         <v>2717</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" ht="42.75">
-      <c r="A13" s="6" t="s">
-        <v>44</v>
+      <c r="A13" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="B13">
         <v>16</v>
@@ -1582,12 +1586,12 @@
         <v>10120558</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" ht="42.75">
-      <c r="A14" s="6" t="s">
-        <v>46</v>
+      <c r="A14" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B14">
         <v>16</v>
@@ -1606,12 +1610,12 @@
         <v>10120862</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" ht="42.75">
-      <c r="A15" s="6" t="s">
-        <v>48</v>
+      <c r="A15" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1627,15 +1631,15 @@
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="6" t="s">
-        <v>51</v>
+      <c r="A16" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="B16">
         <f>3*9+4</f>
@@ -1649,18 +1653,18 @@
         <v>86.489999999999995</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F16" s="1">
         <v>24300</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17">
         <v>9</v>
@@ -1673,18 +1677,18 @@
         <v>2.7450000000000001</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="6" t="s">
-        <v>58</v>
+      <c r="A18" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="B18">
         <v>9</v>
@@ -1697,18 +1701,18 @@
         <v>7.6139999999999999</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1">
         <v>25515</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19">
         <v>16</v>
@@ -1721,13 +1725,13 @@
         <v>24.800000000000001</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="7" t="s">
         <v>63</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="20" ht="14.25">
@@ -1739,12 +1743,12 @@
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G3"/>
-    <hyperlink r:id="rId1" ref="G5"/>
-    <hyperlink r:id="rId2" ref="G9"/>
-    <hyperlink r:id="rId3" ref="E12"/>
-    <hyperlink r:id="rId4" ref="G16"/>
-    <hyperlink r:id="rId5" ref="G18"/>
-    <hyperlink r:id="rId6" ref="G19"/>
+    <hyperlink r:id="rId2" ref="G5"/>
+    <hyperlink r:id="rId3" ref="G9"/>
+    <hyperlink r:id="rId4" ref="E12"/>
+    <hyperlink r:id="rId5" ref="G16"/>
+    <hyperlink r:id="rId6" ref="G18"/>
+    <hyperlink r:id="rId7" ref="G19"/>
   </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>

</xml_diff>

<commit_message>
add an onpi variable to test the dashboard on computer first
</commit_message>
<xml_diff>
--- a/sphinx/source/Ohmpi_V2_00/step_n_3/a/MUX_board_list_2_xx.xlsx
+++ b/sphinx/source/Ohmpi_V2_00/step_n_3/a/MUX_board_list_2_xx.xlsx
@@ -21,10 +21,10 @@
     <t>Number</t>
   </si>
   <si>
-    <t xml:space="preserve">Cost per unit â‚¬ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total cost â‚¬</t>
+    <t xml:space="preserve">Cost per unit (EUR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total cost (EUR)</t>
   </si>
   <si>
     <t>Manufacturer</t>
@@ -69,7 +69,7 @@
     <t xml:space="preserve">Pin strip no ejector  6 pins</t>
   </si>
   <si>
-    <t>https://www.conrad.com/p/tru-components-1580990-pin-strip-no-ejector-contact-spacing-254-mm-total-number-of-pins-6-no-of-rows-2-1-pcs-1580990</t>
+    <t>https://www.conrad.com/p/bkl-electronic-10120550-pin-strip-no-ejector-contact-spacing-254-mm-total-number-of-pins-6-no-of-rows-2-1-pcs-741435</t>
   </si>
   <si>
     <t xml:space="preserve">Dual screw terminal (5.08-mm pitch)</t>
@@ -1343,7 +1343,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="1">
-        <v>10120550</v>
+        <v>1580994</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>
@@ -1391,7 +1391,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1">
-        <v>1580990</v>
+        <v>10120550</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>18</v>

</xml_diff>